<commit_message>
File name edit for csv
</commit_message>
<xml_diff>
--- a/QueryDetails.xlsx
+++ b/QueryDetails.xlsx
@@ -444,10 +444,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -499,6 +499,26 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>SELECT  company_name,reg_id, company_address FROM public."Company"</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Company_1.csv</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>